<commit_message>
devops doc with flow diagram
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SATHIYAVATHI\Desktop\Anandh_Study_material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DB64B3-1B05-44E3-B1DF-EA521BDF4252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FDA12F-0A46-4697-9C11-AC0BCFE15131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3861,16 +3862,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3885,7 +3886,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7229476" y="1638300"/>
+          <a:off x="7743826" y="2133600"/>
           <a:ext cx="933450" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -3934,16 +3935,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3958,7 +3959,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9305926" y="1866900"/>
+          <a:off x="9820276" y="2362200"/>
           <a:ext cx="1209674" cy="390525"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4007,16 +4008,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4031,7 +4032,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8943975" y="2390775"/>
+          <a:off x="9458325" y="2886075"/>
           <a:ext cx="933450" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4080,16 +4081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4104,7 +4105,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8982075" y="2838450"/>
+          <a:off x="9496425" y="3333750"/>
           <a:ext cx="933450" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4153,16 +4154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4177,7 +4178,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8924925" y="3352801"/>
+          <a:off x="9439275" y="3848101"/>
           <a:ext cx="1152525" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4226,16 +4227,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4250,7 +4251,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8886825" y="3819526"/>
+          <a:off x="9401175" y="4314826"/>
           <a:ext cx="1152525" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4299,16 +4300,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4323,7 +4324,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7905750" y="4171951"/>
+          <a:off x="8420100" y="4667251"/>
           <a:ext cx="1152525" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4372,16 +4373,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133351</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4398,7 +4399,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6657975" y="1971675"/>
+          <a:off x="7172325" y="2466975"/>
           <a:ext cx="1038226" cy="857250"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4424,16 +4425,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4448,7 +4449,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6648450" y="2143125"/>
+          <a:off x="7162800" y="2638425"/>
           <a:ext cx="2695575" cy="695326"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4474,16 +4475,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>80963</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>4763</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4500,7 +4501,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6648450" y="2557463"/>
+          <a:off x="7162800" y="3052763"/>
           <a:ext cx="2295525" cy="290512"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4526,16 +4527,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>147638</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4552,7 +4553,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6657975" y="2838450"/>
+          <a:off x="7172325" y="3333750"/>
           <a:ext cx="2324100" cy="166688"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4578,16 +4579,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4604,7 +4605,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6657975" y="2847975"/>
+          <a:off x="7172325" y="3343275"/>
           <a:ext cx="2266950" cy="666751"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4630,16 +4631,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4656,7 +4657,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6648450" y="2857500"/>
+          <a:off x="7162800" y="3352800"/>
           <a:ext cx="2238375" cy="1123951"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4682,16 +4683,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>309563</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4708,7 +4709,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6667500" y="2867025"/>
+          <a:off x="7181850" y="3362325"/>
           <a:ext cx="1814513" cy="1304926"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4734,16 +4735,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>304800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>155448</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504824</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>79248</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4758,7 +4759,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7820025" y="1257300"/>
+          <a:off x="8334375" y="1752600"/>
           <a:ext cx="3390899" cy="612648"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeEllipseCallout">
@@ -4797,16 +4798,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>3048</xdr:rowOff>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>117348</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4821,7 +4822,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9963151" y="2628900"/>
+          <a:off x="10477501" y="3124200"/>
           <a:ext cx="1885950" cy="612648"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeEllipseCallout">
@@ -5496,6 +5497,125 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B79FA37-6AB4-4ED7-9278-615178FC3A36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6791325" y="2438400"/>
+          <a:ext cx="381000" cy="1838325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>11738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1A77BBC-510D-446F-BE36-85A769E7ECCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="6410326"/>
+          <a:ext cx="9877424" cy="3697912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5969,8 +6089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E37C445-2875-4EE6-9E97-653A70D41761}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6021,7 +6141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95558BB-BB72-4CE0-A4A4-133A52B4D3EF}">
   <dimension ref="C3:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>